<commit_message>
stat result 2d 2 1d oop ok.
</commit_message>
<xml_diff>
--- a/data/define/define.xlsx
+++ b/data/define/define.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12540" activeTab="10"/>
+    <workbookView windowWidth="20430" windowHeight="5775" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="metric" sheetId="5" r:id="rId1"/>
@@ -3799,11 +3799,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="0.00_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="32">
     <font>
@@ -3879,38 +3879,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3923,6 +3894,65 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -3931,8 +3961,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3955,40 +3994,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3999,17 +4008,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -4062,7 +4062,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4074,13 +4074,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4092,67 +4092,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4170,7 +4122,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4182,61 +4230,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4332,15 +4332,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -4351,30 +4342,6 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -4410,6 +4377,39 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -4434,148 +4434,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -4616,7 +4616,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5470,7 +5470,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" outlineLevelCol="3"/>
@@ -5728,8 +5728,8 @@
   <sheetPr/>
   <dimension ref="A1:AK81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P40" sqref="P40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -11712,8 +11712,8 @@
   <sheetPr/>
   <dimension ref="A1:D139"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23" defaultRowHeight="16.5" outlineLevelCol="3"/>
@@ -13684,7 +13684,7 @@
   <dimension ref="A1:D92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" outlineLevelCol="3"/>
@@ -18328,8 +18328,8 @@
   <sheetPr/>
   <dimension ref="A1:L139"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -20184,7 +20184,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" outlineLevelCol="6"/>
@@ -20326,7 +20326,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="13" ht="17.25" spans="1:3">
+    <row r="13" spans="1:3">
       <c r="A13" s="24" t="s">
         <v>1008</v>
       </c>

</xml_diff>